<commit_message>
feat: init demo dataset for dashboard dev
</commit_message>
<xml_diff>
--- a/emx2/model/dashboard_emx2.xlsx
+++ b/emx2/model/dashboard_emx2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-rd-erns/emx2/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CADE644-A2D1-FD4C-B120-6D7EEEDFF27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF10776-5C43-C845-937E-BB8FC2C46464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4680" yWindow="-23500" windowWidth="38400" windowHeight="23500" xr2:uid="{A4445CB8-6650-5644-8867-79CD32362061}"/>
+    <workbookView xWindow="-38400" yWindow="-3180" windowWidth="38400" windowHeight="21100" xr2:uid="{A4445CB8-6650-5644-8867-79CD32362061}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="80">
   <si>
     <t>tableName</t>
   </si>
@@ -125,9 +125,6 @@
     <t>inclusionCriteria</t>
   </si>
   <si>
-    <t>Define or modify inclusion criteria for each subgroup</t>
-  </si>
-  <si>
     <t>A unique ID used to identify a group</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>A variable to identify criteria for a specific group (e.g., "genes", "disease", etc.)</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -230,9 +224,6 @@
     <t>An indication that a file, record, or dataset has been sbmitted to a data repository</t>
   </si>
   <si>
-    <t>An inclusion criteria</t>
-  </si>
-  <si>
     <t>https://schema.org/name</t>
   </si>
   <si>
@@ -264,6 +255,27 @@
   </si>
   <si>
     <t>Information about organisations within the context of the project</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25466</t>
+  </si>
+  <si>
+    <t>That which constitutes a standard from which a judgment can be established, a reference point against which other things can be evaluated, or a basis for comparison.</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25284</t>
+  </si>
+  <si>
+    <t>Something distinguishable as an identifiable class based on common qualities</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0500027</t>
+  </si>
+  <si>
+    <t>An inclusion criterion (rule) is_a *eligibility criterion* which defines and states a condition which, if met, makes an entity suitable for a given task or participation in a given process. For instance, in a study protocol, inclusion criteria indicate the conditions that prospective subjects MUST meet to be eligible for participation in a study.</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000947</t>
   </si>
 </sst>
 </file>
@@ -626,11 +638,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD944BE9-CEDB-2647-8189-870C9965A528}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,7 +682,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -683,8 +695,11 @@
       <c r="A2" t="s">
         <v>28</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -704,10 +719,10 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -715,16 +730,16 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -732,13 +747,16 @@
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="K5" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -746,13 +764,16 @@
         <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="K6" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -760,16 +781,16 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -777,33 +798,35 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="K9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -815,29 +838,29 @@
         <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -846,26 +869,26 @@
         <v>13</v>
       </c>
       <c r="J12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -880,157 +903,157 @@
         <v>1</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
         <v>22</v>
       </c>
       <c r="J16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" t="s">
         <v>40</v>
       </c>
-      <c r="E18" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" t="s">
-        <v>42</v>
-      </c>
       <c r="J18" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
@@ -1047,10 +1070,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
         <v>18</v>
@@ -1067,10 +1090,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D25" t="s">
         <v>21</v>
@@ -1087,10 +1110,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
         <v>25</v>
@@ -1107,22 +1130,45 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" t="s">
         <v>59</v>
       </c>
-      <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" t="s">
-        <v>70</v>
-      </c>
-      <c r="H27" t="s">
-        <v>68</v>
-      </c>
-      <c r="I27" t="s">
-        <v>61</v>
+      <c r="J28" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1135,6 +1181,12 @@
     <hyperlink ref="J3" r:id="rId6" xr:uid="{A34B9F43-FB96-DF4E-98FA-8D783BF2699E}"/>
     <hyperlink ref="J10" r:id="rId7" xr:uid="{E0A77E94-4C5F-394D-91C2-E946688482D0}"/>
     <hyperlink ref="J20" r:id="rId8" location="component" xr:uid="{908A80C9-241B-8549-9CCF-70B774948D43}"/>
+    <hyperlink ref="J5" r:id="rId9" xr:uid="{A2FC844A-8BFC-CA40-A5CC-41E665E2D9F1}"/>
+    <hyperlink ref="J6" r:id="rId10" xr:uid="{52116EF7-6817-CA40-B0F8-DBA11F02333F}"/>
+    <hyperlink ref="J27" r:id="rId11" xr:uid="{87FD780B-4487-F847-9E4C-DECD4C780260}"/>
+    <hyperlink ref="J2" r:id="rId12" xr:uid="{2DE8A6F3-74C0-3845-B8D7-4085C5EE4B1C}"/>
+    <hyperlink ref="J9" r:id="rId13" xr:uid="{7BF461F7-AB73-4B41-B994-1A0E3B7E62B5}"/>
+    <hyperlink ref="J28" r:id="rId14" xr:uid="{D35FABCD-3198-D047-85A2-4F07530ED0F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>